<commit_message>
map js and data files
</commit_message>
<xml_diff>
--- a/data/data_available.xlsx
+++ b/data/data_available.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianka\Documents\MSc-Internship\Observatory-of-the-Mountains\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E769BA99-1582-4E87-9ABF-8767FE5DBD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB969C8A-6CDF-4D95-86FB-8370D2C8B0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
   </bookViews>
@@ -2339,7 +2339,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
@@ -2361,10 +2361,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2687,8 +2683,8 @@
   <dimension ref="A1:I195"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B141" sqref="B141"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6565,7 +6561,7 @@
   <dimension ref="B2:S199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6881,7 +6877,7 @@
       <c r="M16" s="16" t="s">
         <v>580</v>
       </c>
-      <c r="N16" s="38"/>
+      <c r="N16" s="15"/>
       <c r="P16" s="14"/>
       <c r="S16" s="14"/>
     </row>
@@ -6964,7 +6960,7 @@
       <c r="B20">
         <v>2024</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>568</v>
       </c>
       <c r="I20" s="13"/>
@@ -7062,7 +7058,7 @@
       <c r="B26">
         <v>2023</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="38" t="s">
         <v>566</v>
       </c>
       <c r="E26">
@@ -7104,7 +7100,7 @@
       <c r="B28">
         <v>2022</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="38" t="s">
         <v>562</v>
       </c>
       <c r="E28">
@@ -7830,6 +7826,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="9050bc6f-8f89-47a3-86fa-b072ef53d328" xsi:nil="true"/>
@@ -7837,7 +7842,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6363AD6CE09334FA2B4FF9AA95D73C5" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="fea41b385c3c40a857800e800f56fbc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9050bc6f-8f89-47a3-86fa-b072ef53d328" xmlns:ns4="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="507616ff13059a37d7288ac12b1b548c" ns3:_="" ns4:_="">
     <xsd:import namespace="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
@@ -8070,16 +8075,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55792E88-4A72-42AB-9F80-0618B4EBFE2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC416A1-3111-4849-A533-05CA95BC2A5C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8096,7 +8100,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13FC5822-06D7-4595-B74F-3FC67EA3A23C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8113,12 +8117,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55792E88-4A72-42AB-9F80-0618B4EBFE2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adjusting the design of the dashboard
</commit_message>
<xml_diff>
--- a/data/data_available.xlsx
+++ b/data/data_available.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianka\Documents\MSc-Internship\Observatory-of-the-Mountains\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB969C8A-6CDF-4D95-86FB-8370D2C8B0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E48FC0-3ABF-4702-B2E3-DA28EECC8A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
   </bookViews>
   <sheets>
     <sheet name="per county" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="586">
   <si>
     <r>
       <t xml:space="preserve">gencat </t>
@@ -1017,9 +1017,6 @@
     <t>https://www.idescat.cat/indicadors/?id=aec&amp;n=15245&amp;tema=xifpo&amp;lang=en</t>
   </si>
   <si>
-    <t>population strucutre by sex and age group</t>
-  </si>
-  <si>
     <t>https://www.idescat.cat/indicadors/?id=aec&amp;n=15233&amp;tema=xifpo&amp;lang=en</t>
   </si>
   <si>
@@ -1694,29 +1691,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>map</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>total aerial biomass</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, total air carbon, volume with bark, foliar biomass, basal area, tree cover, average normal diamter, average heights, leaf area index</t>
     </r>
   </si>
   <si>
@@ -2096,6 +2070,9 @@
       </rPr>
       <t>age group</t>
     </r>
+  </si>
+  <si>
+    <t>total aerial biomass, total air carbon, volume with bark, foliar biomass, basal area, tree cover, average normal diamter, average heights, leaf area index</t>
   </si>
 </sst>
 </file>
@@ -2315,8 +2292,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2325,21 +2311,14 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
@@ -2682,9 +2661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD66C7E-061F-43E9-BB3A-8D29200B2BF1}">
   <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2702,11 +2681,11 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2722,23 +2701,23 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>423</v>
-      </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:9" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="30" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:9" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2764,7 +2743,7 @@
     </row>
     <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -2788,8 +2767,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:9" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2830,8 +2809,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="30" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:9" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2910,8 +2889,8 @@
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>506</v>
+      <c r="B15" s="38" t="s">
+        <v>585</v>
       </c>
       <c r="C15" s="1">
         <v>2005</v>
@@ -2923,31 +2902,31 @@
         <v>2017</v>
       </c>
       <c r="I15" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:9" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>279</v>
       </c>
       <c r="C19" s="1">
         <v>1986</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E19" s="1">
         <v>2024</v>
@@ -2963,15 +2942,15 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="2" t="s">
         <v>282</v>
       </c>
       <c r="C20" s="1">
         <v>1981</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E20" s="1">
         <v>2024</v>
@@ -2987,15 +2966,15 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="30"/>
+      <c r="B21" s="2" t="s">
         <v>284</v>
       </c>
       <c r="C21" s="1">
         <v>1986</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E21" s="1">
         <v>2024</v>
@@ -3011,15 +2990,15 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="1" t="s">
-        <v>286</v>
+        <v>584</v>
       </c>
       <c r="C22" s="1">
         <v>1999</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E22" s="1">
         <v>2024</v>
@@ -3028,19 +3007,19 @@
         <v>47</v>
       </c>
       <c r="I22" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="30"/>
+      <c r="B23" s="1" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="C23" s="1">
         <v>1996</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E23" s="1">
         <v>2021</v>
@@ -3049,22 +3028,22 @@
         <v>47</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="I23" s="4" t="s">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
+      <c r="B24" s="1" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="C24" s="1">
         <v>1996</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E24" s="1">
         <v>2024</v>
@@ -3073,22 +3052,22 @@
         <v>47</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="I24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="30"/>
+      <c r="B25" s="1" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="C25" s="1">
         <v>2004</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E25" s="1">
         <v>2024</v>
@@ -3097,22 +3076,22 @@
         <v>47</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="I25" s="4" t="s">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="1" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="C26" s="1">
         <v>2009</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E26" s="1">
         <v>2025</v>
@@ -3121,22 +3100,22 @@
         <v>47</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I26" s="4" t="s">
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="1" t="s">
         <v>300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="C27" s="1">
         <v>2009</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E27" s="1">
         <v>2025</v>
@@ -3145,24 +3124,24 @@
         <v>47</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="I27" s="4" t="s">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="C28" s="1">
         <v>2000</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E28" s="1">
         <v>2022</v>
@@ -3171,22 +3150,22 @@
         <v>47</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="I28" s="4" t="s">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="1" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
-      <c r="B29" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="C29" s="1">
         <v>1999</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E29" s="1">
         <v>2021</v>
@@ -3195,22 +3174,22 @@
         <v>47</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="I29" s="4" t="s">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="1" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="C30" s="1">
         <v>1999</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E30" s="1">
         <v>2021</v>
@@ -3219,22 +3198,22 @@
         <v>47</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="I30" s="4" t="s">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="1" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="C31" s="1">
         <v>1997</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E31" s="1">
         <v>2022</v>
@@ -3246,19 +3225,19 @@
         <v>162</v>
       </c>
       <c r="I31" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="1" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="C32" s="1">
         <v>1998</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E32" s="1">
         <v>2018</v>
@@ -3267,22 +3246,22 @@
         <v>47</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="I32" s="4" t="s">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="1" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="C33" s="1">
         <v>1999</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E33" s="1">
         <v>2021</v>
@@ -3291,22 +3270,22 @@
         <v>47</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="I33" s="4" t="s">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="30"/>
+      <c r="B34" s="1" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
-      <c r="B34" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="C34" s="1">
         <v>2000</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E34" s="1">
         <v>2024</v>
@@ -3315,46 +3294,46 @@
         <v>47</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="I34" s="4" t="s">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="30"/>
+      <c r="B35" s="1" t="s">
         <v>323</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
-      <c r="B35" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="C35" s="1">
         <v>2000</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E35" s="1">
         <v>2023</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="I35" s="4" t="s">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
+      <c r="B36" s="1" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="C36" s="1">
         <v>2004</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E36" s="1">
         <v>2021</v>
@@ -3363,24 +3342,24 @@
         <v>47</v>
       </c>
       <c r="H36" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="I36" s="4" t="s">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
-        <v>347</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="C37" s="1">
         <v>2002</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E37" s="1">
         <v>2024</v>
@@ -3389,22 +3368,22 @@
         <v>47</v>
       </c>
       <c r="H37" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>333</v>
-      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C38" s="1">
         <v>2002</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E38" s="1">
         <v>2024</v>
@@ -3413,22 +3392,22 @@
         <v>47</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="I38" s="4" t="s">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="1" t="s">
         <v>335</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="C39" s="1">
         <v>2000</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E39" s="1">
         <v>2024</v>
@@ -3437,22 +3416,22 @@
         <v>47</v>
       </c>
       <c r="H39" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="I39" s="4" t="s">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="30"/>
+      <c r="B40" s="1" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="C40" s="1">
         <v>2000</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E40" s="1">
         <v>2024</v>
@@ -3461,22 +3440,22 @@
         <v>47</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I40" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="30"/>
+      <c r="B41" s="1" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="1" t="s">
-        <v>341</v>
       </c>
       <c r="C41" s="1">
         <v>2000</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E41" s="1">
         <v>2024</v>
@@ -3485,22 +3464,22 @@
         <v>47</v>
       </c>
       <c r="H41" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="I41" s="4" t="s">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="30"/>
+      <c r="B42" s="1" t="s">
         <v>343</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
-      <c r="B42" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="C42" s="1">
         <v>1996</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E42" s="1">
         <v>2023</v>
@@ -3509,24 +3488,24 @@
         <v>47</v>
       </c>
       <c r="H42" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="I42" s="4" t="s">
-        <v>346</v>
-      </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="30" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C43" s="1">
         <v>1999</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E43" s="1">
         <v>2019</v>
@@ -3535,22 +3514,22 @@
         <v>47</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C44" s="1">
         <v>2000</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E44" s="1">
         <v>2019</v>
@@ -3559,22 +3538,22 @@
         <v>47</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C45" s="1">
         <v>1999</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E45" s="1">
         <v>2021</v>
@@ -3583,22 +3562,22 @@
         <v>47</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C46" s="1">
         <v>1999</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E46" s="1">
         <v>2019</v>
@@ -3607,24 +3586,24 @@
         <v>47</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="30" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C47" s="1">
         <v>1999</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E47" s="1">
         <v>2023</v>
@@ -3633,22 +3612,22 @@
         <v>143</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>366</v>
-      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C48" s="1">
         <v>2004</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E48" s="1">
         <v>2023</v>
@@ -3657,24 +3636,24 @@
         <v>47</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="I48" t="s">
         <v>362</v>
       </c>
-      <c r="I48" t="s">
-        <v>363</v>
-      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="30" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C49" s="1">
         <v>2000</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E49" s="1">
         <v>2022</v>
@@ -3686,19 +3665,19 @@
         <v>128</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C50" s="1">
         <v>1999</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E50" s="1">
         <v>2015</v>
@@ -3707,22 +3686,22 @@
         <v>143</v>
       </c>
       <c r="H50" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I50" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="I50" s="8" t="s">
-        <v>375</v>
-      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C51" s="1">
         <v>1999</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E51" s="1">
         <v>2023</v>
@@ -3731,22 +3710,22 @@
         <v>47</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="I51" t="s">
         <v>376</v>
       </c>
-      <c r="I51" t="s">
-        <v>377</v>
-      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="33"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C52" s="1">
         <v>2000</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E52" s="1">
         <v>2024</v>
@@ -3755,22 +3734,22 @@
         <v>47</v>
       </c>
       <c r="H52" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I52" t="s">
         <v>378</v>
       </c>
-      <c r="I52" t="s">
-        <v>379</v>
-      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="33"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C53" s="1">
         <v>2000</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E53" s="1">
         <v>2024</v>
@@ -3779,22 +3758,22 @@
         <v>47</v>
       </c>
       <c r="H53" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>381</v>
-      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C54" s="1">
         <v>2000</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E54" s="1">
         <v>2024</v>
@@ -3803,22 +3782,22 @@
         <v>47</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="I54" t="s">
         <v>382</v>
       </c>
-      <c r="I54" t="s">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="30"/>
+      <c r="B55" s="2" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="C55" s="1">
         <v>1996</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E55" s="1">
         <v>2023</v>
@@ -3827,22 +3806,22 @@
         <v>47</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I55" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
-      <c r="B56" s="1" t="s">
-        <v>385</v>
+      <c r="A56" s="30"/>
+      <c r="B56" s="2" t="s">
+        <v>384</v>
       </c>
       <c r="C56" s="1">
         <v>1996</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E56" s="1">
         <v>2023</v>
@@ -3851,14 +3830,14 @@
         <v>47</v>
       </c>
       <c r="H56" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="I56" t="s">
         <v>387</v>
       </c>
-      <c r="I56" t="s">
-        <v>388</v>
-      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="1" t="s">
         <v>80</v>
       </c>
@@ -3866,7 +3845,7 @@
         <v>1996</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E57" s="1">
         <v>2022</v>
@@ -3875,14 +3854,14 @@
         <v>47</v>
       </c>
       <c r="H57" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="I57" t="s">
         <v>389</v>
       </c>
-      <c r="I57" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="1" t="s">
         <v>80</v>
       </c>
@@ -3890,7 +3869,7 @@
         <v>1996</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E58" s="1">
         <v>2022</v>
@@ -3899,14 +3878,14 @@
         <v>47</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I58" t="s">
         <v>391</v>
       </c>
-      <c r="I58" t="s">
-        <v>392</v>
-      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="33"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="1" t="s">
         <v>80</v>
       </c>
@@ -3914,7 +3893,7 @@
         <v>1996</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E59" s="1">
         <v>2022</v>
@@ -3923,14 +3902,14 @@
         <v>47</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I59" s="4" t="s">
-        <v>394</v>
-      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="1" t="s">
         <v>80</v>
       </c>
@@ -3938,7 +3917,7 @@
         <v>1996</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E60" s="1">
         <v>2022</v>
@@ -3947,22 +3926,22 @@
         <v>47</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="I60" t="s">
         <v>395</v>
       </c>
-      <c r="I60" t="s">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="30"/>
+      <c r="B61" s="1" t="s">
         <v>396</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
-      <c r="B61" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="C61" s="1">
         <v>2000</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E61" s="1">
         <v>2022</v>
@@ -3971,22 +3950,22 @@
         <v>47</v>
       </c>
       <c r="H61" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="I61" s="4" t="s">
-        <v>399</v>
-      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
-      <c r="B62" s="1" t="s">
-        <v>402</v>
+      <c r="A62" s="30"/>
+      <c r="B62" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="C62" s="1">
         <v>1999</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E62" s="1">
         <v>2024</v>
@@ -3995,22 +3974,22 @@
         <v>47</v>
       </c>
       <c r="H62" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="I62" t="s">
         <v>400</v>
       </c>
-      <c r="I62" t="s">
-        <v>401</v>
-      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C63" s="1">
         <v>1999</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E63" s="1">
         <v>2023</v>
@@ -4019,19 +3998,19 @@
         <v>47</v>
       </c>
       <c r="H63" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="I63" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="I63" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
+    </row>
+    <row r="65" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="31" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="33" t="s">
+      <c r="A66" s="30" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -4057,7 +4036,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="1" t="s">
         <v>236</v>
       </c>
@@ -4081,7 +4060,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="33"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="1" t="s">
         <v>239</v>
       </c>
@@ -4105,9 +4084,9 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="33"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C69" s="1">
         <v>1990</v>
@@ -4129,7 +4108,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="33"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="1" t="s">
         <v>245</v>
       </c>
@@ -4153,7 +4132,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="33"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="1" t="s">
         <v>248</v>
       </c>
@@ -4161,7 +4140,7 @@
         <v>2001</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E71" s="1">
         <v>2024</v>
@@ -4177,7 +4156,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="33"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="1" t="s">
         <v>250</v>
       </c>
@@ -4185,7 +4164,7 @@
         <v>2000</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E72" s="1">
         <v>2024</v>
@@ -4201,7 +4180,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4211,7 +4190,7 @@
         <v>2000</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E73" s="1">
         <v>2023</v>
@@ -4227,7 +4206,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="1" t="s">
         <v>255</v>
       </c>
@@ -4235,7 +4214,7 @@
         <v>2000</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E74" s="1">
         <v>2023</v>
@@ -4251,7 +4230,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="33"/>
+      <c r="A75" s="30"/>
       <c r="B75" s="1" t="s">
         <v>258</v>
       </c>
@@ -4259,7 +4238,7 @@
         <v>2001</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E75" s="1">
         <v>2024</v>
@@ -4275,7 +4254,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="33"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="1" t="s">
         <v>261</v>
       </c>
@@ -4283,7 +4262,7 @@
         <v>2000</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E76" s="1">
         <v>2024</v>
@@ -4299,7 +4278,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="30"/>
       <c r="B77" s="1" t="s">
         <v>264</v>
       </c>
@@ -4307,7 +4286,7 @@
         <v>2000</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E77" s="1">
         <v>2024</v>
@@ -4323,7 +4302,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="33"/>
+      <c r="A78" s="30"/>
       <c r="B78" s="1" t="s">
         <v>267</v>
       </c>
@@ -4331,7 +4310,7 @@
         <v>1999</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E78" s="1">
         <v>2023</v>
@@ -4347,7 +4326,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="33"/>
+      <c r="A79" s="30"/>
       <c r="B79" s="1" t="s">
         <v>270</v>
       </c>
@@ -4355,7 +4334,7 @@
         <v>2018</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E79" s="1">
         <v>2024</v>
@@ -4371,7 +4350,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="33"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="1" t="s">
         <v>273</v>
       </c>
@@ -4379,7 +4358,7 @@
         <v>2011</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E80" s="1">
         <v>2024</v>
@@ -4395,7 +4374,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="33"/>
+      <c r="A81" s="30"/>
       <c r="B81" s="1" t="s">
         <v>276</v>
       </c>
@@ -4403,7 +4382,7 @@
         <v>2000</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E81" s="1">
         <v>2024</v>
@@ -4418,23 +4397,23 @@
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="30" t="s">
+    <row r="83" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="33" t="s">
+      <c r="A84" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C84" s="1">
         <v>2001</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E84" s="1">
         <v>2022</v>
@@ -4450,15 +4429,15 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="33"/>
-      <c r="B85" s="1" t="s">
+      <c r="A85" s="30"/>
+      <c r="B85" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C85" s="1">
         <v>2006</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E85" s="1">
         <v>2022</v>
@@ -4474,15 +4453,15 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="33"/>
-      <c r="B86" s="1" t="s">
+      <c r="A86" s="30"/>
+      <c r="B86" s="2" t="s">
         <v>199</v>
       </c>
       <c r="C86" s="1">
         <v>2006</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E86" s="1">
         <v>2022</v>
@@ -4498,15 +4477,15 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="33"/>
-      <c r="B87" s="1" t="s">
+      <c r="A87" s="30"/>
+      <c r="B87" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C87" s="1">
         <v>2000</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E87" s="1">
         <v>2022</v>
@@ -4522,15 +4501,15 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="33"/>
-      <c r="B88" s="1" t="s">
+      <c r="A88" s="30"/>
+      <c r="B88" s="2" t="s">
         <v>205</v>
       </c>
       <c r="C88" s="1">
         <v>2000</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E88" s="1">
         <v>2022</v>
@@ -4546,17 +4525,17 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="33" t="s">
+      <c r="A89" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="2" t="s">
         <v>208</v>
       </c>
       <c r="C89" s="1">
         <v>1996</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E89" s="1">
         <v>2024</v>
@@ -4572,15 +4551,15 @@
       </c>
     </row>
     <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="33"/>
-      <c r="B90" s="1" t="s">
+      <c r="A90" s="30"/>
+      <c r="B90" s="2" t="s">
         <v>211</v>
       </c>
       <c r="C90" s="1">
         <v>2002</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E90" s="1">
         <v>2024</v>
@@ -4596,7 +4575,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="33" t="s">
+      <c r="A91" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -4606,7 +4585,7 @@
         <v>1995</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E91" s="1">
         <v>2023</v>
@@ -4619,15 +4598,15 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="33"/>
-      <c r="B92" s="1" t="s">
+      <c r="A92" s="30"/>
+      <c r="B92" s="2" t="s">
         <v>216</v>
       </c>
       <c r="C92" s="1">
         <v>2002</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E92" s="1">
         <v>2022</v>
@@ -4643,7 +4622,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="33"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="1" t="s">
         <v>218</v>
       </c>
@@ -4651,7 +4630,7 @@
         <v>1999</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E93" s="1">
         <v>2024</v>
@@ -4667,7 +4646,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="33"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="1" t="s">
         <v>219</v>
       </c>
@@ -4675,7 +4654,7 @@
         <v>1999</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E94" s="1">
         <v>2024</v>
@@ -4691,7 +4670,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="33"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="1" t="s">
         <v>223</v>
       </c>
@@ -4699,7 +4678,7 @@
         <v>2000</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E95" s="1">
         <v>2022</v>
@@ -4715,7 +4694,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="33" t="s">
+      <c r="A96" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -4725,7 +4704,7 @@
         <v>2005</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E96" s="1">
         <v>2023</v>
@@ -4741,7 +4720,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="33"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="1" t="s">
         <v>229</v>
       </c>
@@ -4749,7 +4728,7 @@
         <v>2005</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E97" s="1">
         <v>2023</v>
@@ -4764,16 +4743,16 @@
         <v>231</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="s">
+    <row r="99" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+      <c r="A100" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="38" t="s">
         <v>71</v>
       </c>
       <c r="C100" s="1">
@@ -4796,7 +4775,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="33"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="1" t="s">
         <v>72</v>
       </c>
@@ -4820,7 +4799,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="33"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="1" t="s">
         <v>74</v>
       </c>
@@ -4844,7 +4823,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="33"/>
+      <c r="A103" s="30"/>
       <c r="B103" s="1" t="s">
         <v>77</v>
       </c>
@@ -4868,7 +4847,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="33"/>
+      <c r="A104" s="30"/>
       <c r="B104" s="1" t="s">
         <v>80</v>
       </c>
@@ -4892,7 +4871,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="33"/>
+      <c r="A105" s="30"/>
       <c r="B105" s="1" t="s">
         <v>84</v>
       </c>
@@ -4916,8 +4895,8 @@
       </c>
     </row>
     <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="33"/>
-      <c r="B106" s="1" t="s">
+      <c r="A106" s="30"/>
+      <c r="B106" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C106" s="1">
@@ -4940,7 +4919,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="33"/>
+      <c r="A107" s="30"/>
       <c r="B107" s="1" t="s">
         <v>90</v>
       </c>
@@ -4964,8 +4943,8 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="33"/>
-      <c r="B108" s="1" t="s">
+      <c r="A108" s="30"/>
+      <c r="B108" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C108" s="1">
@@ -4988,7 +4967,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="33"/>
+      <c r="A109" s="30"/>
       <c r="B109" s="1" t="s">
         <v>97</v>
       </c>
@@ -4996,7 +4975,7 @@
         <v>2020</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E109" s="1">
         <v>2020</v>
@@ -5012,7 +4991,7 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="33" t="s">
+      <c r="A110" s="30" t="s">
         <v>106</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -5022,7 +5001,7 @@
         <v>1999</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E110" s="1">
         <v>2023</v>
@@ -5038,7 +5017,7 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="33"/>
+      <c r="A111" s="30"/>
       <c r="B111" s="1" t="s">
         <v>102</v>
       </c>
@@ -5062,7 +5041,7 @@
       </c>
     </row>
     <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+      <c r="A112" s="30" t="s">
         <v>61</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -5072,7 +5051,7 @@
         <v>2003</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E112" s="1">
         <v>2024</v>
@@ -5088,7 +5067,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="33"/>
+      <c r="A113" s="30"/>
       <c r="B113" s="1" t="s">
         <v>110</v>
       </c>
@@ -5096,7 +5075,7 @@
         <v>2003</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E113" s="1">
         <v>2024</v>
@@ -5112,7 +5091,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="33"/>
+      <c r="A114" s="30"/>
       <c r="B114" s="1" t="s">
         <v>112</v>
       </c>
@@ -5120,7 +5099,7 @@
         <v>1996</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E114" s="1">
         <v>2024</v>
@@ -5136,7 +5115,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="33"/>
+      <c r="A115" s="30"/>
       <c r="B115" s="1" t="s">
         <v>115</v>
       </c>
@@ -5144,7 +5123,7 @@
         <v>2000</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E115" s="1">
         <v>2024</v>
@@ -5160,7 +5139,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="33"/>
+      <c r="A116" s="30"/>
       <c r="B116" s="1" t="s">
         <v>118</v>
       </c>
@@ -5168,7 +5147,7 @@
         <v>2005</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E116" s="1">
         <v>2024</v>
@@ -5184,7 +5163,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="33"/>
+      <c r="A117" s="30"/>
       <c r="B117" s="1" t="s">
         <v>123</v>
       </c>
@@ -5192,7 +5171,7 @@
         <v>2000</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E117" s="1">
         <v>2024</v>
@@ -5208,7 +5187,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="33"/>
+      <c r="A118" s="30"/>
       <c r="B118" s="1" t="s">
         <v>124</v>
       </c>
@@ -5216,7 +5195,7 @@
         <v>2000</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E118" s="1">
         <v>2024</v>
@@ -5232,7 +5211,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="33"/>
+      <c r="A119" s="30"/>
       <c r="B119" s="1" t="s">
         <v>127</v>
       </c>
@@ -5240,7 +5219,7 @@
         <v>2004</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E119" s="1">
         <v>2024</v>
@@ -5256,7 +5235,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="33" t="s">
+      <c r="A120" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -5266,7 +5245,7 @@
         <v>2002</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E120" s="1">
         <v>2023</v>
@@ -5282,7 +5261,7 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="33"/>
+      <c r="A121" s="30"/>
       <c r="B121" s="1" t="s">
         <v>133</v>
       </c>
@@ -5290,7 +5269,7 @@
         <v>2004</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E121" s="1">
         <v>2023</v>
@@ -5306,7 +5285,7 @@
       </c>
     </row>
     <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="33" t="s">
+      <c r="A122" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -5316,7 +5295,7 @@
         <v>2003</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E122" s="1">
         <v>2024</v>
@@ -5332,7 +5311,7 @@
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="33"/>
+      <c r="A123" s="30"/>
       <c r="B123" s="1" t="s">
         <v>139</v>
       </c>
@@ -5340,7 +5319,7 @@
         <v>2000</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E123" s="1">
         <v>2024</v>
@@ -5356,7 +5335,7 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="33"/>
+      <c r="A124" s="30"/>
       <c r="B124" s="1" t="s">
         <v>142</v>
       </c>
@@ -5364,7 +5343,7 @@
         <v>2003</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E124" s="1">
         <v>2024</v>
@@ -5380,7 +5359,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="33"/>
+      <c r="A125" s="30"/>
       <c r="B125" s="1" t="s">
         <v>146</v>
       </c>
@@ -5388,7 +5367,7 @@
         <v>2002</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E125" s="1">
         <v>2024</v>
@@ -5403,13 +5382,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="30" t="s">
+    <row r="127" spans="1:9" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="31" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="33" t="s">
+      <c r="A128" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -5419,7 +5398,7 @@
         <v>2000</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E128" s="1">
         <v>2024</v>
@@ -5435,15 +5414,15 @@
       </c>
     </row>
     <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="33"/>
-      <c r="B129" s="1" t="s">
+      <c r="A129" s="30"/>
+      <c r="B129" s="2" t="s">
         <v>152</v>
       </c>
       <c r="C129" s="1">
         <v>2000</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E129" s="1">
         <v>2024</v>
@@ -5459,15 +5438,15 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="33"/>
-      <c r="B130" s="1" t="s">
+      <c r="A130" s="30"/>
+      <c r="B130" s="2" t="s">
         <v>154</v>
       </c>
       <c r="C130" s="1">
         <v>2002</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E130" s="1">
         <v>2024</v>
@@ -5483,7 +5462,7 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="33"/>
+      <c r="A131" s="30"/>
       <c r="B131" s="1" t="s">
         <v>158</v>
       </c>
@@ -5491,7 +5470,7 @@
         <v>1999</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E131" s="1">
         <v>2023</v>
@@ -5507,15 +5486,15 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="33"/>
-      <c r="B132" s="1" t="s">
+      <c r="A132" s="30"/>
+      <c r="B132" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C132" s="1">
         <v>1998</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E132" s="1">
         <v>2022</v>
@@ -5531,15 +5510,15 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="33"/>
-      <c r="B133" s="1" t="s">
+      <c r="A133" s="30"/>
+      <c r="B133" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C133" s="1">
         <v>1998</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E133" s="1">
         <v>2023</v>
@@ -5555,7 +5534,7 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="33"/>
+      <c r="A134" s="30"/>
       <c r="B134" s="1" t="s">
         <v>166</v>
       </c>
@@ -5563,7 +5542,7 @@
         <v>2000</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E134" s="1">
         <v>2022</v>
@@ -5579,15 +5558,15 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="33"/>
-      <c r="B135" s="1" t="s">
+      <c r="A135" s="30"/>
+      <c r="B135" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C135" s="1">
         <v>2001</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E135" s="1">
         <v>2024</v>
@@ -5603,7 +5582,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="33"/>
+      <c r="A136" s="30"/>
       <c r="B136" s="1" t="s">
         <v>172</v>
       </c>
@@ -5611,7 +5590,7 @@
         <v>2000</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E136" s="1">
         <v>2023</v>
@@ -5627,7 +5606,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="33"/>
+      <c r="A137" s="30"/>
       <c r="B137" s="1" t="s">
         <v>175</v>
       </c>
@@ -5635,7 +5614,7 @@
         <v>1995</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E137" s="1">
         <v>2021</v>
@@ -5651,7 +5630,7 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="33"/>
+      <c r="A138" s="30"/>
       <c r="B138" s="1" t="s">
         <v>178</v>
       </c>
@@ -5659,7 +5638,7 @@
         <v>1995</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E138" s="1">
         <v>2021</v>
@@ -5675,7 +5654,7 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A139" s="33"/>
+      <c r="A139" s="30"/>
       <c r="B139" s="1" t="s">
         <v>181</v>
       </c>
@@ -5683,7 +5662,7 @@
         <v>1995</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E139" s="1">
         <v>2021</v>
@@ -5699,27 +5678,27 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="33" t="s">
+      <c r="A140" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>184</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I140" s="1"/>
     </row>
     <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="33"/>
-      <c r="B141" s="1" t="s">
+      <c r="A141" s="30"/>
+      <c r="B141" s="2" t="s">
         <v>185</v>
       </c>
       <c r="C141" s="1">
         <v>2001</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E141" s="1">
         <v>2023</v>
@@ -5735,19 +5714,19 @@
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="33"/>
+      <c r="A142" s="30"/>
       <c r="B142" s="1" t="s">
         <v>188</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I142" s="4" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="33"/>
+      <c r="A143" s="30"/>
       <c r="B143" s="1" t="s">
         <v>190</v>
       </c>
@@ -5755,7 +5734,7 @@
         <v>2003</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E143" s="1">
         <v>2024</v>
@@ -5767,29 +5746,29 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:9" s="35" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="35" t="s">
+    <row r="145" spans="1:9" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="32" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="30" t="s">
+        <v>416</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>407</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="33" t="s">
-        <v>417</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="C146" s="1">
         <v>2006</v>
       </c>
       <c r="I146" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="33"/>
+      <c r="A147" s="30"/>
       <c r="B147" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C147" s="1">
         <v>2001</v>
@@ -5798,23 +5777,23 @@
         <v>2013</v>
       </c>
       <c r="I147" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="33"/>
+      <c r="A148" s="30"/>
       <c r="B148" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I148" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="33"/>
+      <c r="A149" s="30"/>
       <c r="B149" s="1" t="s">
         <v>158</v>
       </c>
@@ -5825,43 +5804,43 @@
         <v>2023</v>
       </c>
       <c r="H149" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="I149" t="s">
         <v>429</v>
       </c>
-      <c r="I149" t="s">
-        <v>430</v>
-      </c>
     </row>
     <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="33"/>
+      <c r="A150" s="30"/>
       <c r="B150" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C150" s="1">
         <v>2002</v>
       </c>
       <c r="H150" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="I150" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="30"/>
+      <c r="B151" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I150" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="33"/>
-      <c r="B151" s="1" t="s">
+      <c r="C151" s="1">
+        <v>2024</v>
+      </c>
+      <c r="I151" t="s">
         <v>433</v>
       </c>
-      <c r="C151" s="1">
-        <v>2024</v>
-      </c>
-      <c r="I151" t="s">
-        <v>434</v>
-      </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="33"/>
+      <c r="A152" s="30"/>
       <c r="B152" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C152" s="1">
         <v>2006</v>
@@ -5870,51 +5849,51 @@
         <v>2016</v>
       </c>
       <c r="I152" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="33"/>
+      <c r="A153" s="30"/>
       <c r="B153" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C153" s="1">
         <v>2023</v>
       </c>
       <c r="I153" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="33"/>
+      <c r="A154" s="30"/>
       <c r="B154" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C154" s="1">
         <v>2003</v>
       </c>
       <c r="I154" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="33"/>
+      <c r="A155" s="30"/>
       <c r="B155" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C155" s="1">
         <v>2005</v>
       </c>
       <c r="I155" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="C156" s="1">
         <v>1981</v>
@@ -5923,30 +5902,30 @@
         <v>2021</v>
       </c>
       <c r="I156" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="30" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="33" t="s">
-        <v>421</v>
-      </c>
       <c r="B157" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C157" s="1">
         <v>1970</v>
       </c>
       <c r="H157" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="I157" t="s">
         <v>440</v>
       </c>
-      <c r="I157" t="s">
+    </row>
+    <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="30"/>
+      <c r="B158" s="1" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="33"/>
-      <c r="B158" s="1" t="s">
-        <v>442</v>
       </c>
       <c r="C158" s="1">
         <v>2000</v>
@@ -5955,78 +5934,78 @@
         <v>2006</v>
       </c>
       <c r="H158" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I158" t="s">
         <v>443</v>
       </c>
-      <c r="I158" t="s">
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="30"/>
+      <c r="B159" s="1" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="33"/>
-      <c r="B159" s="1" t="s">
-        <v>445</v>
       </c>
       <c r="C159" s="1">
         <v>2008</v>
       </c>
       <c r="I159" s="4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="30"/>
+      <c r="B160" s="1" t="s">
         <v>446</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="33"/>
-      <c r="B160" s="1" t="s">
-        <v>447</v>
       </c>
       <c r="C160" s="1">
         <v>2008</v>
       </c>
       <c r="I160" s="4" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" s="30"/>
+      <c r="B161" s="1" t="s">
         <v>448</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="33"/>
-      <c r="B161" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="C161" s="1">
         <v>2007</v>
       </c>
       <c r="I161" s="4" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162" s="30"/>
+      <c r="B162" s="1" t="s">
         <v>450</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="33"/>
-      <c r="B162" s="1" t="s">
-        <v>451</v>
       </c>
       <c r="C162" s="1">
         <v>2008</v>
       </c>
       <c r="I162" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" s="30"/>
+      <c r="B163" s="1" t="s">
         <v>452</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="33"/>
-      <c r="B163" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="C163" s="1">
         <v>2008</v>
       </c>
       <c r="I163" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" s="30" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="33" t="s">
+      <c r="B164" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>456</v>
       </c>
       <c r="C164" s="1">
         <v>2019</v>
@@ -6035,13 +6014,13 @@
         <v>2024</v>
       </c>
       <c r="I164" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="30"/>
+      <c r="B165" s="1" t="s">
         <v>457</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A165" s="33"/>
-      <c r="B165" s="1" t="s">
-        <v>458</v>
       </c>
       <c r="C165" s="1">
         <v>2008</v>
@@ -6051,11 +6030,11 @@
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" s="33" t="s">
+      <c r="A166" s="30" t="s">
+        <v>458</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="C166" s="1">
         <v>2002</v>
@@ -6064,30 +6043,30 @@
         <v>2012</v>
       </c>
       <c r="I166" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" s="30"/>
+      <c r="B167" s="1" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="33"/>
-      <c r="B167" s="1" t="s">
+      <c r="C167" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E167" s="1">
+        <v>2024</v>
+      </c>
+      <c r="I167" t="s">
         <v>462</v>
       </c>
-      <c r="C167" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E167" s="1">
-        <v>2024</v>
-      </c>
-      <c r="I167" t="s">
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" s="30" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="33" t="s">
+      <c r="B168" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="C168" s="1">
         <v>2019</v>
@@ -6096,13 +6075,13 @@
         <v>2019</v>
       </c>
       <c r="I168" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="33"/>
+      <c r="A169" s="30"/>
       <c r="B169" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C169" s="1">
         <v>2023</v>
@@ -6111,15 +6090,15 @@
         <v>2023</v>
       </c>
       <c r="I169" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="30" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="33" t="s">
+      <c r="B170" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="C170" s="1">
         <v>2012</v>
@@ -6132,13 +6111,13 @@
       </c>
       <c r="H170" s="7"/>
       <c r="I170" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="33"/>
+      <c r="A171" s="30"/>
       <c r="B171" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C171" s="1">
         <v>2016</v>
@@ -6149,16 +6128,16 @@
       <c r="H171" s="7"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A172" s="33"/>
+      <c r="A172" s="30"/>
       <c r="B172" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="H172" s="7"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173" s="30"/>
+      <c r="B173" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="H172" s="7"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A173" s="33"/>
-      <c r="B173" s="1" t="s">
-        <v>472</v>
       </c>
       <c r="C173" s="1">
         <v>2019</v>
@@ -6169,16 +6148,16 @@
       <c r="H173" s="7"/>
     </row>
     <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="33"/>
+      <c r="A174" s="30"/>
       <c r="B174" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="H174" s="7"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175" s="30"/>
+      <c r="B175" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="H174" s="7"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A175" s="33"/>
-      <c r="B175" s="1" t="s">
-        <v>474</v>
       </c>
       <c r="C175" s="1">
         <v>2019</v>
@@ -6189,9 +6168,9 @@
       <c r="H175" s="7"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A176" s="33"/>
+      <c r="A176" s="30"/>
       <c r="B176" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C176" s="1">
         <v>2019</v>
@@ -6202,9 +6181,9 @@
       <c r="H176" s="7"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" s="33"/>
+      <c r="A177" s="30"/>
       <c r="B177" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C177" s="1">
         <v>2019</v>
@@ -6215,9 +6194,9 @@
       <c r="H177" s="7"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" s="33"/>
+      <c r="A178" s="30"/>
       <c r="B178" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C178" s="1">
         <v>2019</v>
@@ -6228,11 +6207,11 @@
       <c r="H178" s="7"/>
     </row>
     <row r="179" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="33" t="s">
+      <c r="A179" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="B179" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>480</v>
       </c>
       <c r="C179" s="1">
         <v>2020</v>
@@ -6242,13 +6221,13 @@
       </c>
       <c r="H179" s="7"/>
       <c r="I179" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" s="33"/>
+      <c r="A180" s="30"/>
       <c r="B180" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C180" s="1">
         <v>2020</v>
@@ -6259,9 +6238,9 @@
       <c r="H180" s="7"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="33"/>
+      <c r="A181" s="30"/>
       <c r="B181" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C181" s="1">
         <v>2020</v>
@@ -6272,9 +6251,9 @@
       <c r="H181" s="7"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" s="33"/>
+      <c r="A182" s="30"/>
       <c r="B182" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C182" s="1">
         <v>2020</v>
@@ -6285,9 +6264,9 @@
       <c r="H182" s="7"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="33"/>
+      <c r="A183" s="30"/>
       <c r="B183" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C183" s="1">
         <v>2020</v>
@@ -6298,9 +6277,9 @@
       <c r="H183" s="7"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="33"/>
+      <c r="A184" s="30"/>
       <c r="B184" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C184" s="1">
         <v>2020</v>
@@ -6311,9 +6290,9 @@
       <c r="H184" s="7"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="33"/>
+      <c r="A185" s="30"/>
       <c r="B185" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C185" s="1">
         <v>2020</v>
@@ -6324,9 +6303,9 @@
       <c r="H185" s="7"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="33"/>
+      <c r="A186" s="30"/>
       <c r="B186" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C186" s="1">
         <v>2020</v>
@@ -6337,9 +6316,9 @@
       <c r="H186" s="7"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="33"/>
+      <c r="A187" s="30"/>
       <c r="B187" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C187" s="1">
         <v>2020</v>
@@ -6350,9 +6329,9 @@
       <c r="H187" s="7"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" s="33"/>
+      <c r="A188" s="30"/>
       <c r="B188" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C188" s="1">
         <v>2020</v>
@@ -6363,9 +6342,9 @@
       <c r="H188" s="7"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="33"/>
+      <c r="A189" s="30"/>
       <c r="B189" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C189" s="1">
         <v>2020</v>
@@ -6376,9 +6355,9 @@
       <c r="H189" s="7"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="33"/>
+      <c r="A190" s="30"/>
       <c r="B190" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C190" s="1">
         <v>2020</v>
@@ -6390,10 +6369,10 @@
     </row>
     <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C191" s="1">
         <v>2019</v>
@@ -6402,18 +6381,18 @@
         <v>2019</v>
       </c>
       <c r="H191" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I191" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" s="33" t="s">
-        <v>496</v>
+      <c r="A192" s="30" t="s">
+        <v>495</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C192" s="1">
         <v>2008</v>
@@ -6422,27 +6401,27 @@
         <v>2020</v>
       </c>
       <c r="H192" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="I192" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="I192" s="8" t="s">
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="30"/>
+      <c r="B193" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="33"/>
-      <c r="B193" s="1" t="s">
+      <c r="I193" t="s">
         <v>499</v>
       </c>
-      <c r="I193" t="s">
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>500</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>501</v>
       </c>
       <c r="C194" s="1">
         <v>2009</v>
@@ -6451,32 +6430,42 @@
         <v>2012</v>
       </c>
       <c r="I194" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="30"/>
+      <c r="B195" s="1" t="s">
         <v>502</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" s="33"/>
-      <c r="B195" s="1" t="s">
-        <v>503</v>
       </c>
       <c r="C195" s="1">
         <v>2010</v>
       </c>
       <c r="I195" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="E1:E195" xr:uid="{1CD66C7E-061F-43E9-BB3A-8D29200B2BF1}"/>
   <mergeCells count="40">
-    <mergeCell ref="A179:A190"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="A157:A163"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="A170:A178"/>
+    <mergeCell ref="A83:XFD83"/>
+    <mergeCell ref="A99:XFD99"/>
+    <mergeCell ref="A3:XFD3"/>
+    <mergeCell ref="A17:XFD17"/>
+    <mergeCell ref="A49:A63"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A73:A81"/>
+    <mergeCell ref="A65:XFD65"/>
+    <mergeCell ref="A19:A27"/>
+    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A4:XFD4"/>
+    <mergeCell ref="A7:XFD7"/>
+    <mergeCell ref="A10:XFD10"/>
+    <mergeCell ref="A18:XFD18"/>
     <mergeCell ref="A146:A155"/>
     <mergeCell ref="A84:A88"/>
     <mergeCell ref="A89:A90"/>
@@ -6491,24 +6480,14 @@
     <mergeCell ref="A122:A125"/>
     <mergeCell ref="A128:A139"/>
     <mergeCell ref="A140:A143"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A4:XFD4"/>
-    <mergeCell ref="A7:XFD7"/>
-    <mergeCell ref="A10:XFD10"/>
-    <mergeCell ref="A18:XFD18"/>
-    <mergeCell ref="A83:XFD83"/>
-    <mergeCell ref="A99:XFD99"/>
-    <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="A17:XFD17"/>
-    <mergeCell ref="A49:A63"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A73:A81"/>
-    <mergeCell ref="A65:XFD65"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="A28:A36"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A179:A190"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="A157:A163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="A168:A169"/>
+    <mergeCell ref="A170:A178"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I61" r:id="rId1" xr:uid="{551A33CD-200A-4B76-8CDC-E646EC35A9E5}"/>
@@ -6560,7 +6539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27833425-745A-496A-BBBC-9D84991CFB19}">
   <dimension ref="B2:S199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+    <sheetView zoomScale="88" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -6584,20 +6563,20 @@
   <sheetData>
     <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="27" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="26" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="37" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="M2" s="27" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="36"/>
@@ -6605,34 +6584,34 @@
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="19" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="11"/>
       <c r="C4" s="24" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="24" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="20" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="21" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="16" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="S4" s="14"/>
     </row>
@@ -6647,7 +6626,7 @@
         <v>2024</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I5" s="13"/>
       <c r="L5">
@@ -6669,7 +6648,7 @@
         <v>2024</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="I6" s="13"/>
       <c r="L6">
@@ -6685,7 +6664,7 @@
         <v>2024</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E7">
         <v>2024</v>
@@ -6701,7 +6680,7 @@
         <v>2024</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E8">
         <v>2024</v>
@@ -6711,12 +6690,12 @@
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="21" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="16" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="S8" s="14"/>
     </row>
@@ -6725,7 +6704,7 @@
         <v>2024</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I9" s="13"/>
       <c r="L9">
@@ -6741,15 +6720,15 @@
         <v>2024</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="24" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I10" s="13"/>
       <c r="S10" s="14"/>
@@ -6759,22 +6738,22 @@
         <v>2025</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E11">
         <v>2024</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="21" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="16" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="S11" s="14"/>
     </row>
@@ -6783,13 +6762,13 @@
         <v>2025</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E12">
         <v>2024</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I12" s="13"/>
       <c r="L12">
@@ -6806,17 +6785,17 @@
         <v>2024</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="21" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="L13">
         <v>2024</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="O13" s="3"/>
       <c r="S13" s="14"/>
@@ -6824,20 +6803,20 @@
     <row r="14" spans="2:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="24" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E14">
         <v>2024</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="I14" s="13"/>
       <c r="L14">
         <v>2020</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="O14" s="3"/>
       <c r="S14" s="14"/>
@@ -6847,13 +6826,13 @@
         <v>2022</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E15">
         <v>2024</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I15" s="13"/>
       <c r="S15" s="14"/>
@@ -6863,19 +6842,19 @@
         <v>2022</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E16">
         <v>2023</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16"/>
       <c r="L16" s="12"/>
       <c r="M16" s="16" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="N16" s="15"/>
       <c r="P16" s="14"/>
@@ -6892,7 +6871,7 @@
         <v>2023</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17"/>
@@ -6900,7 +6879,7 @@
         <v>2022</v>
       </c>
       <c r="M17" s="15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="N17" s="15"/>
       <c r="P17" s="14"/>
@@ -6925,7 +6904,7 @@
         <v>2021</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="N18" s="15"/>
       <c r="P18" s="14"/>
@@ -6936,13 +6915,13 @@
         <v>2022</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E19">
         <v>2024</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19"/>
@@ -6950,7 +6929,7 @@
         <v>2019</v>
       </c>
       <c r="M19" s="15" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="N19" s="15"/>
       <c r="P19" s="14"/>
@@ -6961,7 +6940,7 @@
         <v>2024</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="I20" s="13"/>
       <c r="S20" s="14"/>
@@ -6974,16 +6953,16 @@
         <v>214</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="21" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="16" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -6992,21 +6971,21 @@
         <v>2020</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="23" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="24" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="25" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="20" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I23" s="13"/>
       <c r="L23">
@@ -7021,7 +7000,7 @@
         <v>2023</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E24">
         <v>2024</v>
@@ -7036,7 +7015,7 @@
         <v>2023</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E25">
         <v>2022</v>
@@ -7046,20 +7025,20 @@
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="21" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="16" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2023</v>
       </c>
-      <c r="C26" s="38" t="s">
-        <v>566</v>
+      <c r="C26" s="15" t="s">
+        <v>564</v>
       </c>
       <c r="E26">
         <v>2023</v>
@@ -7072,7 +7051,7 @@
         <v>2024</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -7080,41 +7059,41 @@
         <v>2024</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E27">
         <v>2020</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I27" s="13"/>
       <c r="L27">
         <v>2020</v>
       </c>
       <c r="M27" s="17" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2022</v>
       </c>
-      <c r="C28" s="38" t="s">
-        <v>562</v>
+      <c r="C28" s="15" t="s">
+        <v>560</v>
       </c>
       <c r="E28">
         <v>2020</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I28" s="13"/>
       <c r="L28">
         <v>2020</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
@@ -7122,14 +7101,14 @@
         <v>2020</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I29" s="13"/>
       <c r="L29">
         <v>2020</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
@@ -7139,13 +7118,13 @@
         <v>2020</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="E31" s="10"/>
       <c r="F31" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I31" s="13"/>
     </row>
@@ -7154,7 +7133,7 @@
         <v>2020</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I32" s="13"/>
     </row>
@@ -7163,7 +7142,7 @@
         <v>2024</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="I33" s="13"/>
     </row>
@@ -7172,7 +7151,7 @@
         <v>2024</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I34" s="13"/>
     </row>
@@ -7182,11 +7161,11 @@
     <row r="36" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E36" s="10"/>
       <c r="F36" s="24" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="20" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="I36" s="13"/>
     </row>
@@ -7196,11 +7175,11 @@
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E38" s="10"/>
       <c r="F38" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="20" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="I38" s="13"/>
     </row>
@@ -7209,7 +7188,7 @@
         <v>2020</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="I39" s="13"/>
     </row>
@@ -7227,7 +7206,7 @@
         <v>2020</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="I41" s="13"/>
     </row>
@@ -7236,7 +7215,7 @@
         <v>2020</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="I42" s="13"/>
     </row>
@@ -7245,7 +7224,7 @@
         <v>2020</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="I43" s="13"/>
     </row>
@@ -7263,7 +7242,7 @@
         <v>2020</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="I45" s="13"/>
     </row>
@@ -7274,7 +7253,7 @@
     <row r="47" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E47" s="10"/>
       <c r="F47" s="24" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="20" t="s">
@@ -7287,7 +7266,7 @@
         <v>2024</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I48" s="13"/>
     </row>
@@ -7296,7 +7275,7 @@
         <v>2023</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I49" s="13"/>
     </row>
@@ -7305,11 +7284,11 @@
         <v>2024</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I50" s="13"/>
       <c r="J50" s="28" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="51" spans="5:10" ht="30" x14ac:dyDescent="0.25">
@@ -7317,11 +7296,11 @@
         <v>2024</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="28" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="52" spans="5:10" ht="30" x14ac:dyDescent="0.25">
@@ -7329,11 +7308,11 @@
         <v>2024</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="28" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.25">
@@ -7341,7 +7320,7 @@
         <v>2024</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I53" s="13"/>
     </row>
@@ -7350,7 +7329,7 @@
         <v>2024</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I54" s="13"/>
     </row>
@@ -7361,11 +7340,11 @@
     <row r="56" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E56" s="10"/>
       <c r="F56" s="24" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G56" s="10"/>
       <c r="H56" s="20" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="I56" s="13"/>
     </row>
@@ -7374,7 +7353,7 @@
         <v>2023</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I57" s="13"/>
     </row>
@@ -7383,7 +7362,7 @@
         <v>2019</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I58" s="13"/>
     </row>
@@ -7392,25 +7371,25 @@
     </row>
     <row r="60" spans="5:10" ht="30" x14ac:dyDescent="0.25">
       <c r="H60" s="29" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="5:10" x14ac:dyDescent="0.25">
       <c r="H61" s="29" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I61" s="13"/>
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.25">
       <c r="H62" s="29" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I62" s="13"/>
     </row>
     <row r="63" spans="5:10" x14ac:dyDescent="0.25">
       <c r="H63" s="29" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I63" s="13"/>
     </row>
@@ -7835,14 +7814,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9050bc6f-8f89-47a3-86fa-b072ef53d328" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6363AD6CE09334FA2B4FF9AA95D73C5" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="fea41b385c3c40a857800e800f56fbc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9050bc6f-8f89-47a3-86fa-b072ef53d328" xmlns:ns4="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="507616ff13059a37d7288ac12b1b548c" ns3:_="" ns4:_="">
     <xsd:import namespace="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
@@ -8075,6 +8046,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9050bc6f-8f89-47a3-86fa-b072ef53d328" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55792E88-4A72-42AB-9F80-0618B4EBFE2A}">
   <ds:schemaRefs>
@@ -8084,23 +8063,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC416A1-3111-4849-A533-05CA95BC2A5C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13FC5822-06D7-4595-B74F-3FC67EA3A23C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8117,4 +8079,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC416A1-3111-4849-A533-05CA95BC2A5C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>